<commit_message>
added pause to verify good generation
</commit_message>
<xml_diff>
--- a/python3.6/PIP_GEN_id-0/ConsoleProcedures.xlsx
+++ b/python3.6/PIP_GEN_id-0/ConsoleProcedures.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420"/>
   </bookViews>
   <sheets>
     <sheet name="english" sheetId="2" r:id="rId1"/>
@@ -1904,10 +1904,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U1" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -36219,9 +36219,9 @@
   <dimension ref="A1:AF1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -70517,7 +70517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added lock/unlock and "CONSOLE" socket steps
</commit_message>
<xml_diff>
--- a/python3.6/PIP_GEN_id-0/ConsoleProcedures.xlsx
+++ b/python3.6/PIP_GEN_id-0/ConsoleProcedures.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="258">
   <si>
     <t>LINK</t>
   </si>
@@ -239,14 +239,6 @@
 Verify that the Incline on the console and EQF1259 match.</t>
   </si>
   <si>
-    <t xml:space="preserve">Press the iFIT sync button and verify a 4 character Hex in the middle of the display (Example: “DF69”). 
-Tap the Bluetooth icon on the top right of tablet screen
-In the pop up window, tap your machine choice and verify signal strength at 0.5m is (&gt;50%)
-Tap “OKAY”. The Bluetooth icon in the upper right of the tablet display will blink and then go solid blue. The console will show connection indicator.
-Tap the Bluetooth icon on the upper right on tablet screen and “UNPAIR” the console.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Connect the power cord to the EQF1259. 
 Connect one end of the EQW1001 to EQF1259 (BIKE2). NOTE: MAKE SURE YOU SELECT THE CORRECT PORT THAT MATCH THE TYPE OF THE CONSOLE.   
 Set Fixture Configurations:
@@ -419,13 +411,6 @@
   <si>
     <t>Touch gear icon at the lower center  of the screen.
 Touch "Maintainance". This will display App version and Brainboard version.
-Verify and Record.
-Press the back arrow on the tablet to return to main screen</t>
-  </si>
-  <si>
-    <t>Touch user profile icon at the lower right  of the screen
-Touch settings
-Touch “Equipment Info” and then “App Info”. This will display App version and Brainboard version.
 Verify and Record.
 Press the back arrow on the tablet to return to main screen</t>
   </si>
@@ -619,11 +604,6 @@
 </t>
   </si>
   <si>
-    <t>On the EQF1259, turn off the Console power.
-Remove batteries from console
-Disconnect all wires and cables from the console.</t>
-  </si>
-  <si>
     <t>“将电源线连接到EQF1259，将EQW1001的一端连接到EQF1259（TRED1）。注意：请确保您选择与控制台类型相匹配的正确端口。将地线（绿色）连接到E-GND EQF 1259.设置夹具配置：使用PC，在控制台名称（例如：... RNDFtp \ EBNT02117 \ Procedure）下载入RNDftp中的.xml配置文件到microSD卡，将microSD卡正面朝上插入microSD打开灯具背面的RESET按钮，使用UP和DOWN按钮找到合适的配置文件，按ENTER键选择配置文件（屏幕1），等待5秒钟，屏幕稳定后设置灯具脉冲：按下EQF1259 2x上的显示按下此灯具上的开始使用上下按钮设置一个随机脉冲，按下灯具上的开始，按下显示一次。</t>
   </si>
   <si>
@@ -697,9 +677,6 @@
   </si>
   <si>
     <t>将死者的钥匙插入控制台。</t>
-  </si>
-  <si>
-    <t>“按iFIT同步按钮，在显示屏中间验证一个4字符的十六进制（例如：”DF69“）。点击平板电脑屏幕右上方的蓝牙图标在弹出的窗口中，点击您的机器选择并验证信号点击“确定”，平板显示器右上方的蓝牙图标将闪烁，然后变为蓝色，控制台将显示连接指示灯，点击右上角的蓝牙图标平板电脑屏幕和“UNPAIR”控制台。</t>
   </si>
   <si>
     <t>通过IPC-A-610标准仔细检查PCB。请注意PCB上的焊接引脚，焊桥，焊锡飞溅物和异物。</t>
@@ -911,11 +888,6 @@
   </si>
   <si>
     <t>“在EQF1259上，关闭控制台电源。
-断开控制台上的所有电线和电缆。“</t>
-  </si>
-  <si>
-    <t>“在EQF1259上，关闭控制台电源。
-从控制台上取下电池
 断开控制台上的所有电线和电缆。“</t>
   </si>
   <si>
@@ -1184,14 +1156,6 @@
 Connect headphones and adjust volume to minimum and maximum and verify a change.</t>
   </si>
   <si>
-    <t>Connect video source to TV
-Connect EQWxxxx harness to the TV and other end to back of console
-Connect  EQWxxxx harness to the TV and other end to back of console
-Turn on TV with console controls and play video source on TV
-Audio will play through the console speakers
-Adjust TV audio volume on console and the function will display on the TV and the console audio will reflect change</t>
-  </si>
-  <si>
     <t xml:space="preserve">note:
 Press the STOP button while inserting the SAFETY Key. Verify the language is ENGLISH. Use SPEED ^ to change the language between ENGLISH and METRIC. 
 Press STOP, the screen will show “PRESS INCLINE UP OR DOWN TO CALIBARTE”.
@@ -1415,6 +1379,157 @@
   </si>
   <si>
     <t>BL</t>
+  </si>
+  <si>
+    <t>Lock console by press and holding the Ifit button (SYNC) and the Resistance (GEAR) increase and decrease for 3 seconds
+Verify that "Hello" or "ifit.com/activate" is displayed
+On the EQF1259, turn off the Console power.
+Remove batteries from console
+Disconnect all wires and cables from the console.</t>
+  </si>
+  <si>
+    <t>Lock console by press and holding the Ifit button (SYNC) and the Speed increase and decrease for 3 seconds
+Verify that "Hello" or "ifit.com/activate" is displayed
+On the EQF1259, turn off the Console power.
+Disconnect all wires and cables from the console.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If console displays  "Hello" or "ifit.com/activate", press and hold the iFit (SYNC) button for 10 seconds
+Press the iFIT sync button and verify a 4 character Hex in the middle of the display (Example: “DF69”). 
+Tap the Bluetooth icon on the top right of tablet screen
+In the pop up window, tap your machine choice and verify signal strength at 0.5m is (&gt;50%)
+Tap “OKAY”. The Bluetooth icon in the upper right of the tablet display will blink and then go solid blue. The console will show connection indicator.
+Tap the Bluetooth icon on the upper right on tablet screen and “UNPAIR” the console.
+</t>
+  </si>
+  <si>
+    <t>“如果控制台显示”“Hello”“或”“ifit.com/activate”“，请按住iFit（SYNC）按钮10秒钟
+按iFIT同步按钮并在显示屏中间验证4个字符的十六进制（例如：“DF69”）。
+点击平板电脑屏幕右上方的蓝牙图标
+在弹出的窗口中，点击您的机器选择并验证信号强度为0.5m（&gt; 50％）
+点击“OKAY”。 数位板显示屏右上方的蓝牙图标将闪烁，然后变为稳定的蓝色。 控制台将显示连接指示器。
+点击平板电脑屏幕右上方的蓝牙图标和控制台的“UNPAIR”。
+“</t>
+  </si>
+  <si>
+    <t>“按下并按住Ifit按钮（同步）并且速度增加和减少3秒钟以锁定控制台
+验证是否显示“”Hello“”或“”ifit.com/activate“”
+在EQF1259上，关闭控制台电源。
+断开控制台上的所有电线和电缆。“</t>
+  </si>
+  <si>
+    <t>按下并保持“Ifit”按钮（SYNC）和电阻（GEAR）增加和减少3秒钟以锁定控制台
+验证是否显示“你好”或“ifit.com/activate”
+在EQF1259上，关闭控制台电源。
+从控制台上取下电池
+断开控制台上的所有电线和电缆。</t>
+  </si>
+  <si>
+    <t>Clear cache by touch the user profile icon on lower right of the screen
+Touch Settings
+Touch Maintainance
+Touch Clear App Cache and select "YES" and "WELCOME" will appear on display
+Wait 10 seconds and then on the EQF1259, turn off the Console power.
+Disconnect all wires and cables from the console.</t>
+  </si>
+  <si>
+    <t>“通过触摸屏幕右下方的用户配置文件图标清除缓存
+触摸设置
+触摸维护
+触摸Clear App Cache并选择“”YES“”和“”WELCOME“”将出现在显示屏上
+等待10秒钟，然后在EQF1259上关闭控制台电源。
+断开控制台上的所有电线和电缆。“</t>
+  </si>
+  <si>
+    <t>Rev3</t>
+  </si>
+  <si>
+    <r>
+      <t>If console displays  "WELCOME" touch the iFit logo "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>›</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"
+Touch "SKIP"
+Touch "Continue without signing in"
+Touch "SKIP"
+Touch user profile icon at the lower right  of the screen
+Touch settings
+Touch “Equipment Info” and then “App Info”. This will display App version and Brainboard version.
+Verify and Record.
+Press the back arrow on the tablet to return to main screen</t>
+    </r>
+  </si>
+  <si>
+    <t>Lock console by press and holding the Ifit button (SYNC) and the Speed/Resistance increase and decrease for 3 seconds
+Verify that "Hello" or "ifit.com/activate" is displayed
+To unlock BLE console, press the iFit (SYNC) button for ten seconds.</t>
+  </si>
+  <si>
+    <t>Connect video source to TV
+Connect EQWxxxx to the TV and other end to back of console
+Connect  EQWxxxx harness to the TV and other end to back of console
+Turn on TV with console controls and play video source on TV
+Audio will play through the console speakers
+Adjust TV audio volume on console and the function will display on the TV and the console audio will reflect change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connect the power cord to the EQF1259. 
+Connect EQWxxxx male dc to male dc power adapter cable  to EQF1259 (CONSOLE). NOTE: MAKE SURE YOU SELECT THE CORRECT PORT THAT MATCH THE TYPE OF THE CONSOLE.   
+Set Fixture Configurations:
+Using PC, load .xml configuration file, which is found in the RNDftp under the console name (Example: …RNDFtp\EBNT02117\Procedure) to the microSD card.
+Insert the microSD card face up into the microSD card slot.
+Turn on the RESET button at the back of the fixture.
+Using the UP and DOWN buttons locate the proper configuration file.
+Press ENTER to select the configuration file (Screen 1).
+Wait for 5 seconds, when the screen is stable as below.
+Set Fixture Pulse:
+Press Display on the EQF1259 2x.
+Press Start on this fixture
+Using the up and down buttons, set a random pulse.
+Press Start on the fixture.
+Press Display once.
+</t>
+  </si>
+  <si>
+    <t>Connect EQWxxxx male dc to male dc power adapter cable. On the EQF1259, turn on the Console power switch.</t>
+  </si>
+  <si>
+    <t>“将电源线连接到EQF1259。
+将EQWxxxx公头直流电连接到公头直流电源适配器电缆连接到EQF1259（CONSOLE）。 注：请确保您选择与控制台类型相匹配的正确端口。
+设置夹具配置：
+使用PC，在控制台名称下（例如：... RNDFtp \ EBNT02117 \ Procedure），在RNDftp中加载.xml配置文件到microSD卡。
+将microSD卡正面朝上插入microSD卡插槽。
+打开灯具背面的RESET按钮。
+使用UP和DOWN按钮找到正确的配置文件。
+按ENTER键选择配置文件（屏幕1）。
+等待5秒钟，屏幕稳定如下。
+设置灯具脉冲：
+按下EQF1259 2x上的显示。
+按下此灯具上的开始
+使用向上和向下按钮，设置一个随机脉冲。
+按下夹具上的开始。
+按一次显示。
+“</t>
+  </si>
+  <si>
+    <t>将EQWxxxx公头直流连接到公头直流电源适配器电缆。 在EQF1259上，打开控制台电源开关。</t>
+  </si>
+  <si>
+    <t>Added clear cache and BLE lock.
+Added "CONSOLE" socket steps.</t>
   </si>
 </sst>
 </file>
@@ -1905,9 +2020,9 @@
   <dimension ref="A1:AF1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U1" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1945,7 +2060,7 @@
         <v>2</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K1" s="9" t="s">
         <v>4</v>
@@ -1975,7 +2090,7 @@
         <v>7</v>
       </c>
       <c r="T1" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U1" s="9" t="s">
         <v>9</v>
@@ -1999,13 +2114,13 @@
         <v>18</v>
       </c>
       <c r="AB1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AD1" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="AD1" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
@@ -2015,7 +2130,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>24</v>
@@ -2033,22 +2148,22 @@
         <v>30</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>45</v>
+        <v>243</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>80</v>
+        <v>250</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N2" s="11"/>
       <c r="O2" s="12" t="s">
@@ -2067,35 +2182,35 @@
         <v>32</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U2" s="4" t="s">
         <v>36</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="W2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="X2" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y2" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="Y2" s="13" t="s">
-        <v>68</v>
-      </c>
       <c r="Z2" s="14"/>
-      <c r="AA2" s="4" t="s">
-        <v>39</v>
+      <c r="AA2" s="16" t="s">
+        <v>247</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
@@ -2105,7 +2220,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>25</v>
@@ -2117,19 +2232,19 @@
         <v>29</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M3" s="11"/>
       <c r="N3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -2137,22 +2252,22 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>37</v>
       </c>
       <c r="V3" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W3" s="11" t="s">
-        <v>214</v>
+        <v>252</v>
       </c>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="11"/>
-      <c r="AA3" s="4" t="s">
-        <v>96</v>
+      <c r="AA3" s="16" t="s">
+        <v>39</v>
       </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
@@ -2165,7 +2280,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>27</v>
@@ -2175,19 +2290,19 @@
       <c r="F4" s="4"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="11"/>
       <c r="K4" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M4" s="11"/>
       <c r="N4" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -2195,19 +2310,21 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="U4" s="11"/>
       <c r="V4" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="W4" s="11" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="X4" s="4"/>
       <c r="Y4" s="11"/>
       <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
+      <c r="AA4" s="4" t="s">
+        <v>242</v>
+      </c>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
@@ -2219,31 +2336,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="4"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -2251,17 +2368,19 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="U5" s="1"/>
       <c r="V5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="4"/>
       <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
+      <c r="AA5" s="4" t="s">
+        <v>241</v>
+      </c>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
@@ -2273,10 +2392,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2286,16 +2405,16 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="17" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -2303,7 +2422,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U6" s="1"/>
       <c r="X6" s="1"/>
@@ -2321,10 +2440,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -2334,16 +2453,16 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="L7" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="N7" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -2369,31 +2488,31 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="4"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -2419,31 +2538,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="4"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -2469,17 +2588,17 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="4"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -2511,10 +2630,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -2551,10 +2670,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -2591,10 +2710,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2631,10 +2750,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -2671,10 +2790,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2711,14 +2830,18 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>253</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>254</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -2747,7 +2870,7 @@
     <row r="17" spans="1:32" ht="57" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="16" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2783,7 +2906,7 @@
     <row r="18" spans="1:32" ht="57" customHeight="1">
       <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2819,7 +2942,7 @@
     <row r="19" spans="1:32" ht="57" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2855,7 +2978,7 @@
     <row r="20" spans="1:32" ht="57" customHeight="1">
       <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -36219,9 +36342,9 @@
   <dimension ref="A1:AF1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -36313,13 +36436,13 @@
         <v>18</v>
       </c>
       <c r="AB1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AD1" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="AD1" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
@@ -36329,87 +36452,87 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>111</v>
+      <c r="F2" s="4" t="s">
+        <v>109</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>122</v>
+        <v>244</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="S2" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="T2" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="Q2" s="5" t="s">
-        <v>147</v>
+      <c r="U2" s="3" t="s">
+        <v>151</v>
       </c>
-      <c r="R2" s="4" t="s">
-        <v>148</v>
+      <c r="V2" s="6" t="s">
+        <v>153</v>
       </c>
-      <c r="S2" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="U2" s="3" t="s">
+      <c r="W2" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="X2" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="W2" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="Y2" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="Z2" s="1"/>
       <c r="AA2" s="4" t="s">
-        <v>163</v>
+        <v>248</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
@@ -36419,52 +36542,52 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I3" s="1"/>
       <c r="K3" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="T3" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="V3" s="16" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
@@ -36477,46 +36600,48 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="H4" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="V4" s="16" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
+      <c r="AA4" s="1" t="s">
+        <v>245</v>
+      </c>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
@@ -36528,31 +36653,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -36560,17 +36685,19 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="U5" s="4"/>
       <c r="V5" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
+      <c r="AA5" s="1" t="s">
+        <v>246</v>
+      </c>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
@@ -36582,10 +36709,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -36595,16 +36722,16 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="16" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -36612,7 +36739,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="U6" s="1"/>
       <c r="W6" s="1"/>
@@ -36631,10 +36758,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -36644,16 +36771,16 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -36679,29 +36806,29 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -36724,31 +36851,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -36774,17 +36901,17 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -36816,10 +36943,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -36856,10 +36983,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -36895,10 +37022,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -36935,10 +37062,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -36975,10 +37102,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -37015,14 +37142,18 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>255</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>256</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -37051,7 +37182,7 @@
     <row r="17" spans="1:32" ht="57" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -37087,7 +37218,7 @@
     <row r="18" spans="1:32" ht="57" customHeight="1">
       <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -37123,7 +37254,7 @@
     <row r="19" spans="1:32" ht="57" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -37159,7 +37290,7 @@
     <row r="20" spans="1:32" ht="57" customHeight="1">
       <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -70515,69 +70646,86 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B1">
         <v>20180116</v>
       </c>
-      <c r="C1" t="s">
-        <v>127</v>
+      <c r="C1" s="16" t="s">
+        <v>123</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B2">
         <v>20180120</v>
       </c>
-      <c r="C2" t="s">
-        <v>110</v>
+      <c r="C2" s="16" t="s">
+        <v>107</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="409.5">
+    <row r="3" spans="1:9" ht="409.5">
       <c r="A3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B3">
         <v>20180312</v>
       </c>
-      <c r="C3" t="s">
-        <v>245</v>
+      <c r="C3" s="16" t="s">
+        <v>239</v>
       </c>
       <c r="D3" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>215</v>
+      <c r="G3" s="16" t="s">
+        <v>209</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>239</v>
+      <c r="H3" s="16" t="s">
+        <v>233</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="G11" t="s">
-        <v>126</v>
+      <c r="I3" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="51">
+      <c r="A4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B4">
+        <v>20180402</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="D4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="I11" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated location of BLE finish step
</commit_message>
<xml_diff>
--- a/python3.6/PIP_GEN_id-0/ConsoleProcedures.xlsx
+++ b/python3.6/PIP_GEN_id-0/ConsoleProcedures.xlsx
@@ -16,12 +16,12 @@
     <sheet name="chinese" sheetId="3" r:id="rId2"/>
     <sheet name="Revision" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" calcOnSave="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="266">
   <si>
     <t>LINK</t>
   </si>
@@ -192,14 +192,6 @@
     <t>Plug USB cable from EQF1259 into console and verify "USB" is displayed on the EQF1259.</t>
   </si>
   <si>
-    <t>On the EQF1259, Press START.
-Verify that the Cadence(RPM) on the console and the EQF1259 match.</t>
-  </si>
-  <si>
-    <t>On the console, press random Quick speed buttons.
-Verify that the Speed on the console and EQF1259 match.</t>
-  </si>
-  <si>
     <t>On the console, press the RESISTANCE + button. Verify the resistance level on the EQF1259 increases.  
 On the console, press the RESISTANCE - button. Verify the resistance level on the EQF1259 decreases.</t>
   </si>
@@ -257,21 +249,6 @@
 </t>
   </si>
   <si>
-    <t>Connect the 8-pin MTA to console. On the EQF1259, turn on the Console power switch.</t>
-  </si>
-  <si>
-    <t>Connect the 12-pin MTA to console. On the EQF1259, turn on the Console power switch.</t>
-  </si>
-  <si>
-    <t>Connect the 4-pin MTA to console. On the EQF1259, turn on the Console power switch.</t>
-  </si>
-  <si>
-    <t>Connect the 14-pin MTA to console. On the EQF1259, turn on the Console power switch.</t>
-  </si>
-  <si>
-    <t>Connect the 8-pin MTA to console. Insert batteries into console and on the EQF1259, turn on the Console power switch.</t>
-  </si>
-  <si>
     <t>IPC-A-610</t>
   </si>
   <si>
@@ -295,9 +272,6 @@
     <t>BLE CONNECT</t>
   </si>
   <si>
-    <t>Connect the 5-pin MTA to console. Insert batteries into console and on the EQF1259, turn on the Console power switch.</t>
-  </si>
-  <si>
     <t>PULSE TEST</t>
   </si>
   <si>
@@ -305,12 +279,6 @@
   </si>
   <si>
     <t>Press thumb onto the thumb pulse button and verify a pulse reading is displayed</t>
-  </si>
-  <si>
-    <t>Press Display button to goto BLE Pulse screen.
-Press Start button.
-Run manual workout on the console.
-Verify pulse BLE pulse is read on console.</t>
   </si>
   <si>
     <t>Connect the EQW1007 to the iOS audio source and connect the other end of the EQW1007 to the console.
@@ -658,24 +626,6 @@
     <t>检查控制台是否与图片一致如果数位板倾斜，验证倾斜是否平稳移动，保持位置，并旋转全程。</t>
   </si>
   <si>
-    <t>将8针MTA连接到控制台。在EQF1259上，打开控制台电源开关。</t>
-  </si>
-  <si>
-    <t>将12针MTA连接到控制台。在EQF1259上，打开控制台电源开关。</t>
-  </si>
-  <si>
-    <t>将4针MTA连接到控制台。在EQF1259上，打开控制台电源开关。</t>
-  </si>
-  <si>
-    <t>将14针MTA连接到控制台。在EQF1259上，打开控制台电源开关。</t>
-  </si>
-  <si>
-    <t>将5针MTA连接到控制台。将电池插入控制台和EQF1259上，打开控制台电源开关。</t>
-  </si>
-  <si>
-    <t>将8针MTA连接到控制台。将电池插入控制台和EQF1259上，打开控制台电源开关。</t>
-  </si>
-  <si>
     <t>将死者的钥匙插入控制台。</t>
   </si>
   <si>
@@ -801,14 +751,6 @@
 按停止返回主屏幕“</t>
   </si>
   <si>
-    <t>“在控制台上，按随机快速按钮。
-验证控制台上的速度和EQF1259匹配。“</t>
-  </si>
-  <si>
-    <t>“在EQF1259上按START（开始）。
-验证控制台上的Cadence（RPM）和EQF1259匹配。“</t>
-  </si>
-  <si>
     <t>“在控制台上，按随机快速倾斜按钮。
 验证控制台上的倾斜和EQF1259匹配。“</t>
   </si>
@@ -827,18 +769,6 @@
   </si>
   <si>
     <t>用拇指轻轻摩擦传感器，显示心率</t>
-  </si>
-  <si>
-    <t>按显示按钮转到BLE脉冲屏幕。
-按开始按钮。
-点击控制台上的IFIT同步按钮。
-验证在控制台上读取脉冲BLE脉冲。</t>
-  </si>
-  <si>
-    <t>按显示按钮，进入BLE脉冲屏幕。
-按开始按钮。
-在控制台上运行手动锻炼。
-验证在控制台上读取脉冲BLE脉冲。“</t>
   </si>
   <si>
     <t>“在控制台上，按大风扇按钮打开风扇，风扇应该低速运行。
@@ -1005,13 +935,6 @@
   <si>
     <t>Run manual workout on the console.
 Gently rub the sensors with your thumbs will a heart rate displays</t>
-  </si>
-  <si>
-    <t>Press Display button to goto BLE Pulse screen.
-Press Start button.
-Run manual workout on the console.
-Tap the IFIT sync button on the console.
-Verify pulse BLE pulse is read on console.</t>
   </si>
   <si>
     <t>EQF1259 Console Fixture
@@ -1314,26 +1237,6 @@
 Note that the Start and Calibrate buttons are disabled if the console power switch is off.</t>
   </si>
   <si>
-    <t>Connect the 10-pin MTA to console.
-If testing a console with batteries, be absolutely sure the console power switch is off before installing batteries and that the batteries have a good voltage.   Test half sample with batteries. See warnings. 
-Warning!  DO NOT INSTALL BATTERIES INTO A CONSOLE WITH THE CONSOLE POWER SWITCH ON!  THIS MAY CAUSE BATTERIES TO CHARGE AND EXPLODE.
-Warning!  DO NOT INSTALL BATTERIES THAT HAVE A COMBINED VOLTAGE LESS THAN 2 VOLTS. THIS MAY CAUSE BATTERIES TO CHARGE AND EXPLODE.
-Battery test: Once batteries are installed, the Console Power LED will light regardless of the console switch position indicating the console had power. 
-When turning on the console power switch, the EQF1259 checks the console voltage line and if more than 2 volts is detected, the EQF1259 assumes the console is powered by batteries and does not turn on power to the console voltage wires.  The word “Bat” will appear in the top right corner of the display and the EQF1259 will provide signals to the console.
-VDC adapter test: Connect the VDC adapter to console
-On the EQF1259, turn on the Console power switch.</t>
-  </si>
-  <si>
-    <t>“将10针MTA连接到控制台。
-如果使用电池测试控制台，请确保在安装电池之前控制台电源开关已关闭，并且电池电压良好。用电池测试一半样品。见警告。
-警告！不要将电池安装到控制台电源开关的控制台上！这可能会导致电池充电和爆炸。
-警告！请勿安装组合电压低于2伏的电池。这可能会导致电池充电和爆炸。
-电池测试：一旦安装了电池，无论控制台开关位置如何，控制台电源指示灯都会亮起，表示控制台已通电。
-打开控制台电源开关时，EQF1259检查控制台电压线，如果检测到2伏以上，EQF1259假定控制台由电池供电，并且不打开控制台电压线的电源。屏幕右上角将出现“Bat”字样，EQF1259将向控制台提供信号。
-VDC适配器测试：将VDC适配器连接到控制台
-在EQF1259上，打开控制台电源开关。“</t>
-  </si>
-  <si>
     <t xml:space="preserve">Connect the power cord to the EQF1259. 
 Connect one end of the EQW1139 to EQF1259 (BIKE1). NOTE: MAKE SURE YOU SELECT THE CORRECT PORT THAT MATCH THE TYPE OF THE CONSOLE.
 Connect one end of the VDC adapter to "CONSOLE" socket on the EQF1259
@@ -1504,9 +1407,6 @@
 </t>
   </si>
   <si>
-    <t>Connect EQWxxxx male dc to male dc power adapter cable. On the EQF1259, turn on the Console power switch.</t>
-  </si>
-  <si>
     <t>“将电源线连接到EQF1259。
 将EQWxxxx公头直流电连接到公头直流电源适配器电缆连接到EQF1259（CONSOLE）。 注：请确保您选择与控制台类型相匹配的正确端口。
 设置夹具配置：
@@ -1525,11 +1425,204 @@
 “</t>
   </si>
   <si>
-    <t>将EQWxxxx公头直流连接到公头直流电源适配器电缆。 在EQF1259上，打开控制台电源开关。</t>
+    <t>Added clear cache and BLE lock.
+Added "CONSOLE" socket steps.</t>
   </si>
   <si>
-    <t>Added clear cache and BLE lock.
-Added "CONSOLE" socket steps.</t>
+    <t>Start manual workout on the console
+On the EQF1259, Press START.
+Verify that the Cadence(RPM) on the console and the EQF1259 match.</t>
+  </si>
+  <si>
+    <t>“在控制台上开始手动锻炼
+在EQF1259上按START（开始）。
+验证控制台上的Cadence（RPM）和EQF1259匹配。“</t>
+  </si>
+  <si>
+    <t>Rev4</t>
+  </si>
+  <si>
+    <t>Start manual workout on the console.
+On the console, press random Quick speed buttons.
+Verify that the Speed on the console and EQF1259 match.</t>
+  </si>
+  <si>
+    <t>“在控制台上开始手动锻炼。
+在控制台上，按随机快速按钮。
+验证控制台和EQF1259上的速度是否匹配。“</t>
+  </si>
+  <si>
+    <t>On the EQF1259, press Display button to goto BLE Pulse screen.
+Press Start button.
+Run manual workout on the console.
+Tap the IFIT sync button on the console.
+Verify pulse BLE pulse is read on console.</t>
+  </si>
+  <si>
+    <t>On the EQF1259, press Display button to goto BLE Pulse screen.
+Press Start button.
+Run manual workout on the console.
+Verify pulse BLE pulse is read on console.</t>
+  </si>
+  <si>
+    <t>“在EQF1259上，按显示按钮转到BLE脉冲屏幕。
+按下开始按钮。
+在控制台上运行手动锻炼。
+点击控制台上的IFIT同步按钮。
+验证在控制台上读取脉冲BLE脉冲。“</t>
+  </si>
+  <si>
+    <t>“在EQF1259上，按显示按钮转到BLE脉冲屏幕。
+按下开始按钮。
+在控制台上运行手动锻炼。
+验证在控制台上读取脉冲BLE脉冲。“</t>
+  </si>
+  <si>
+    <t>Minor changes to verbage.</t>
+  </si>
+  <si>
+    <t>Connect if needed; pulse bar/grips, speakers, fans, TV, etc.
+Connect the 8-pin MTA to console.
+On the EQF1259, turn on the Console power switch.</t>
+  </si>
+  <si>
+    <t>Connect if needed; pulse bar/grips, speakers, fans, TV, etc.
+Connect the 12-pin MTA to console.
+On the EQF1259, turn on the Console power switch.</t>
+  </si>
+  <si>
+    <t>Connect if needed; pulse bar/grips, speakers, fans, TV, etc.
+Connect the 4-pin MTA to console.
+On the EQF1259, turn on the Console power switch.</t>
+  </si>
+  <si>
+    <t>Connect if needed; pulse bar/grips, speakers, fans, TV, etc.
+Connect the 14-pin MTA to console.
+On the EQF1259, turn on the Console power switch.</t>
+  </si>
+  <si>
+    <t>Connect if needed; pulse bar/grips, speakers, fans, TV, etc.
+Connect the 5-pin MTA to console.
+Insert batteries into console and on the EQF1259, turn on the Console power switch.</t>
+  </si>
+  <si>
+    <t>Connect if needed; pulse bar/grips, speakers, fans, TV, etc.
+Connect the 10-pin MTA to console.
+If testing a console with batteries, be absolutely sure the console power switch is off before installing batteries and that the batteries have a good voltage.   Test half sample with batteries. See warnings. 
+Warning!  DO NOT INSTALL BATTERIES INTO A CONSOLE WITH THE CONSOLE POWER SWITCH ON!  THIS MAY CAUSE BATTERIES TO CHARGE AND EXPLODE.
+Warning!  DO NOT INSTALL BATTERIES THAT HAVE A COMBINED VOLTAGE LESS THAN 2 VOLTS. THIS MAY CAUSE BATTERIES TO CHARGE AND EXPLODE.
+Battery test: Once batteries are installed, the Console Power LED will light regardless of the console switch position indicating the console had power. 
+When turning on the console power switch, the EQF1259 checks the console voltage line and if more than 2 volts is detected, the EQF1259 assumes the console is powered by batteries and does not turn on power to the console voltage wires.  The word “Bat” will appear in the top right corner of the display and the EQF1259 will provide signals to the console.
+VDC adapter test: Connect the VDC adapter to console
+On the EQF1259, turn on the Console power switch.</t>
+  </si>
+  <si>
+    <t>Connect if needed; pulse bar/grips, speakers, fans, TV, etc.
+Connect the 8-pin MTA to console.
+Insert batteries into console and on the EQF1259, turn on the Console power switch.</t>
+  </si>
+  <si>
+    <t>“如果需要连接;脉冲条/手柄，扬声器，风扇，电视等。
+将8针MTA连接到控制台。
+在EQF1259上，打开控制台电源开关。“</t>
+  </si>
+  <si>
+    <t>“如果需要连接;脉冲条/手柄，扬声器，风扇，电视等。
+将12针MTA连接到控制台。
+在EQF1259上，打开控制台电源开关。“</t>
+  </si>
+  <si>
+    <t>“如果需要连接;脉冲条/手柄，扬声器，风扇，电视等。
+将4针MTA连接到控制台。
+在EQF1259上，打开控制台电源开关。“</t>
+  </si>
+  <si>
+    <t>“如果需要连接;脉冲条/手柄，扬声器，风扇，电视等。
+将14针MTA连接到控制台。
+在EQF1259上，打开控制台电源开关。“</t>
+  </si>
+  <si>
+    <t>“如果需要连接;脉冲条/手柄，扬声器，风扇，电视等。
+将5针MTA连接到控制台。
+将电池插入控制台和EQF1259上，打开控制台电源开关。“</t>
+  </si>
+  <si>
+    <t>“如果需要连接;脉冲条/手柄，扬声器，风扇，电视等。
+将10针MTA连接到控制台。
+如果使用电池测试控制台，请确保在安装电池之前控制台电源开关已关闭，并且电池电压良好。用电池测试一半样品。见警告。
+警告！不要将电池安装到控制台电源开关的控制台上！这可能会导致电池充电和爆炸。
+警告！请勿安装组合电压低于2伏的电池。这可能会导致电池充电和爆炸。
+电池测试：一旦安装了电池，无论控制台开关位置如何，控制台电源指示灯都会亮起，表示控制台已通电。
+打开控制台电源开关时，EQF1259会检查控制台电压线，如果检测到2伏以上，则EQF1259假定控制台由电池供电，并且不打开控制台电压线的电源。屏幕右上角将出现“Bat”字样，EQF1259将向控制台提供信号。
+VDC适配器测试：将VDC适配器连接到控制台
+在EQF1259上，打开控制台电源开关。“</t>
+  </si>
+  <si>
+    <t>“如果需要连接;脉冲条/手柄，扬声器，风扇，电视等。
+将8针MTA连接到控制台。
+将电池插入控制台和EQF1259上，打开控制台电源开关。“</t>
+  </si>
+  <si>
+    <t>Connect if needed; pulse bar/grips, speakers, fans, TV, etc.
+Connect EQWxxxx male dc to male dc power adapter cable to the back of the console.
+On the EQF1259, turn on the Console power switch.</t>
+  </si>
+  <si>
+    <t>“如果需要连接;脉冲条/手柄，扬声器，风扇，电视等。
+将EQWxxxx公头直流电源连接到公头直流电源适配器电缆连接到控制台背面。
+在EQF1259上，打开控制台电源开关。“</t>
+  </si>
+  <si>
+    <t>Connect if needed; pulse bar/grips, speakers, fans, TV, etc.
+Connect the 8-pin DIN connector to console.
+On the EQF1259, turn on the Console power switch.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connect the power cord to the EQF1259. 
+Connect one end of the EQW1084 to EQF1259 (RS-485). NOTE: MAKE SURE YOU SELECT THE CORRECT PORT THAT MATCH THE TYPE OF THE CONSOLE.   
+Set Fixture Configurations:
+Using PC, load .xml configuration file, which is found in the RNDftp under the console name (Example: …RNDFtp\EBNT02117\Procedure) to the microSD card.
+Insert the microSD card face up into the microSD card slot.
+Turn on the RESET button at the back of the fixture.
+Using the UP and DOWN buttons locate the proper configuration file.
+Press ENTER to select the configuration file (Screen 1).
+Wait for 5 seconds, when the screen is stable as below.
+Set Fixture Pulse:
+Press Display on the EQF1259 2x.
+Press Start on this fixture
+Using the up and down buttons, set a random pulse.
+Press Start on the fixture.
+Press Display once.
+</t>
+  </si>
+  <si>
+    <t>“将电源线连接到EQF1259。
+将EQW1084的一端连接到EQF1259（RS-485）。 注：请确保您选择与控制台类型相匹配的正确端口。
+设置夹具配置：
+使用PC，在控制台名称下（例如：... RNDFtp \ EBNT02117 \ Procedure），在RNDftp中加载.xml配置文件到microSD卡。
+将microSD卡正面朝上插入microSD卡插槽。
+打开灯具背面的RESET按钮。
+使用UP和DOWN按钮找到正确的配置文件。
+按ENTER键选择配置文件（屏幕1）。
+等待5秒钟，屏幕稳定如下。
+设置灯具脉冲：
+按下EQF1259 2x上的显示。
+按下此灯具上的开始
+使用向上和向下按钮，设置一个随机脉冲。
+按下夹具上的开始。
+按一次显示。
+“</t>
+  </si>
+  <si>
+    <t>“如果需要连接;脉冲条/手柄，扬声器，风扇，电视等。
+将8针DIN连接器连接到控制台。
+在EQF1259上，打开控制台电源开关。“</t>
+  </si>
+  <si>
+    <t>Rev5</t>
+  </si>
+  <si>
+    <t>Added 8-pin DIN harness</t>
   </si>
 </sst>
 </file>
@@ -2019,10 +2112,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U1" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -2060,7 +2153,7 @@
         <v>2</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="K1" s="9" t="s">
         <v>4</v>
@@ -2075,13 +2168,13 @@
         <v>6</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R1" s="9" t="s">
         <v>8</v>
@@ -2090,7 +2183,7 @@
         <v>7</v>
       </c>
       <c r="T1" s="9" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="U1" s="9" t="s">
         <v>9</v>
@@ -2114,13 +2207,13 @@
         <v>18</v>
       </c>
       <c r="AB1" s="9" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="AC1" s="9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="AD1" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
@@ -2130,7 +2223,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>24</v>
@@ -2139,7 +2232,7 @@
         <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>26</v>
@@ -2148,69 +2241,69 @@
         <v>30</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>46</v>
+        <v>244</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>243</v>
+        <v>221</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>250</v>
+        <v>228</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="N2" s="11"/>
       <c r="O2" s="12" t="s">
-        <v>34</v>
+        <v>237</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>33</v>
+        <v>234</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>32</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="U2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="W2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="V2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="X2" s="13" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="Y2" s="13" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="Z2" s="14"/>
       <c r="AA2" s="16" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
@@ -2220,7 +2313,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>25</v>
@@ -2232,19 +2325,19 @@
         <v>29</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>47</v>
+        <v>245</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="M3" s="11"/>
       <c r="N3" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -2252,23 +2345,20 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="V3" s="11" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="W3" s="11" t="s">
-        <v>252</v>
+        <v>230</v>
       </c>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="11"/>
-      <c r="AA3" s="16" t="s">
-        <v>39</v>
-      </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
@@ -2280,7 +2370,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>27</v>
@@ -2290,19 +2380,19 @@
       <c r="F4" s="4"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>48</v>
+        <v>246</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="11"/>
       <c r="K4" s="4" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="M4" s="11"/>
       <c r="N4" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -2310,20 +2400,20 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="U4" s="11"/>
       <c r="V4" s="1" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="W4" s="11" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="X4" s="4"/>
       <c r="Y4" s="11"/>
       <c r="Z4" s="1"/>
-      <c r="AA4" s="4" t="s">
-        <v>242</v>
+      <c r="AA4" s="16" t="s">
+        <v>37</v>
       </c>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
@@ -2336,31 +2426,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="4"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>49</v>
+        <v>247</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="11" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -2368,18 +2458,18 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1" t="s">
-        <v>178</v>
+        <v>239</v>
       </c>
       <c r="U5" s="1"/>
       <c r="V5" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="4"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="4" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
@@ -2392,10 +2482,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2405,16 +2495,16 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="17" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -2422,13 +2512,15 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1" t="s">
-        <v>62</v>
+        <v>240</v>
       </c>
       <c r="U6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
+      <c r="AA6" s="4" t="s">
+        <v>219</v>
+      </c>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
@@ -2440,10 +2532,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -2453,16 +2545,16 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="4" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -2488,31 +2580,31 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="4"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>58</v>
+        <v>248</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="4" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -2538,31 +2630,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>236</v>
+        <v>214</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="4"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="4" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -2588,17 +2680,17 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="4"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -2630,10 +2722,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -2670,16 +2762,15 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="4"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -2710,10 +2801,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2750,10 +2841,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -2790,10 +2881,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2830,17 +2921,17 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>253</v>
+        <v>231</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -2870,14 +2961,18 @@
     <row r="17" spans="1:32" ht="57" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="16" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>261</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>260</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -2906,7 +3001,7 @@
     <row r="18" spans="1:32" ht="57" customHeight="1">
       <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2942,7 +3037,7 @@
     <row r="19" spans="1:32" ht="57" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2978,7 +3073,7 @@
     <row r="20" spans="1:32" ht="57" customHeight="1">
       <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -36341,10 +36436,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -36397,13 +36492,13 @@
         <v>6</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R1" s="9" t="s">
         <v>8</v>
@@ -36436,13 +36531,13 @@
         <v>18</v>
       </c>
       <c r="AB1" s="9" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="AC1" s="9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="AD1" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
@@ -36452,87 +36547,87 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="K2" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>124</v>
-      </c>
       <c r="L2" s="15" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="4" t="s">
-        <v>141</v>
+        <v>238</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>142</v>
+        <v>235</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="Z2" s="1"/>
       <c r="AA2" s="4" t="s">
-        <v>248</v>
+        <v>226</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
@@ -36542,53 +36637,50 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>113</v>
+        <v>252</v>
       </c>
       <c r="I3" s="1"/>
       <c r="K3" s="2" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="T3" s="4" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="V3" s="16" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
-      <c r="AA3" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
@@ -36600,47 +36692,47 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="H4" s="4" t="s">
-        <v>114</v>
+        <v>253</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="4" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="V4" s="16" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1" t="s">
-        <v>245</v>
+        <v>140</v>
       </c>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
@@ -36653,31 +36745,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="4" t="s">
-        <v>115</v>
+        <v>254</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -36685,18 +36777,18 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1" t="s">
-        <v>149</v>
+        <v>241</v>
       </c>
       <c r="U5" s="4"/>
       <c r="V5" s="1" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
@@ -36709,10 +36801,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -36722,16 +36814,16 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="16" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -36739,14 +36831,16 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1" t="s">
-        <v>150</v>
+        <v>242</v>
       </c>
       <c r="U6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
+      <c r="AA6" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
@@ -36758,10 +36852,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -36771,16 +36865,16 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -36806,29 +36900,29 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>116</v>
+        <v>255</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -36851,31 +36945,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>237</v>
+        <v>215</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>235</v>
+        <v>256</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="4" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -36901,17 +36995,17 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>117</v>
+        <v>257</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -36943,10 +37037,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -36983,10 +37077,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -37022,10 +37116,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -37062,10 +37156,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -37102,10 +37196,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -37142,17 +37236,17 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -37182,14 +37276,18 @@
     <row r="17" spans="1:32" ht="57" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>262</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -37218,7 +37316,7 @@
     <row r="18" spans="1:32" ht="57" customHeight="1">
       <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -37254,7 +37352,7 @@
     <row r="19" spans="1:32" ht="57" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -37290,7 +37388,7 @@
     <row r="20" spans="1:32" ht="57" customHeight="1">
       <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -70648,8 +70746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -70660,72 +70758,100 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B1">
         <v>20180116</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B2">
         <v>20180120</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="409.5">
       <c r="A3" t="s">
-        <v>238</v>
+        <v>216</v>
       </c>
       <c r="B3">
         <v>20180312</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="51">
       <c r="A4" t="s">
-        <v>249</v>
+        <v>227</v>
       </c>
       <c r="B4">
         <v>20180402</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="D4" t="s">
-        <v>240</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5">
+        <v>20180410</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>264</v>
+      </c>
+      <c r="B6">
+        <v>20180417</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="D6" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="I11" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>